<commit_message>
#8 Handle local named ranges
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="10560" yWindow="3140" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
-    <sheet name="Taul2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="john">Taul1!$G$7:$M$16</definedName>
-    <definedName name="noncont">Taul1!$19:$19,Taul1!$21:$21</definedName>
-    <definedName name="numbers">Taul1!$C$3:$C$9</definedName>
-    <definedName name="sheet2">Taul2!$B$3:$D$9</definedName>
+    <definedName name="john">Sheet1!$G$7:$M$16</definedName>
+    <definedName name="local" localSheetId="0">Sheet1!$G$2:$H$3</definedName>
+    <definedName name="noncont">Sheet1!$19:$19,Sheet1!$21:$21</definedName>
+    <definedName name="numbers">Sheet1!$C$3:$C$9</definedName>
+    <definedName name="sheet2">Sheet2!$B$3:$D$9</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">       </t>
   </si>
@@ -50,6 +51,9 @@
   <si>
     <t>sheet2</t>
   </si>
+  <si>
+    <t>Local Sheet1 range</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +99,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -108,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -117,6 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Norm." xfId="0" builtinId="0"/>
@@ -397,7 +408,7 @@
   <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G2" sqref="G2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,12 +420,18 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="4">
         <v>4</v>
       </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C4" s="4">

</xml_diff>

<commit_message>
show in the formula bar only those named ranges that can be selected
Contains a workaround for the POI issue https://bz.apache.org/bugzilla/show_bug.cgi?id=61701 that causes IllegalArgumentException when trying to select a named range referring to some formulas.

Jira: SHEET-338
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="3140" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
   <definedNames>
     <definedName name="john">Sheet1!$G$7:$M$16</definedName>
     <definedName name="local" localSheetId="0">Sheet1!$G$2:$H$3</definedName>
+    <definedName name="named_formula">SUM(Sheet1!$C$3:$C$9)</definedName>
     <definedName name="noncont">Sheet1!$19:$19,Sheet1!$21:$21</definedName>
     <definedName name="numbers">Sheet1!$C$3:$C$9</definedName>
     <definedName name="sheet2">Sheet2!$B$3:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -130,13 +131,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -404,19 +408,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -425,7 +429,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="4">
         <v>4</v>
@@ -433,22 +437,22 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C4" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C5" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C6" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C7" s="4">
         <v>9</v>
       </c>
@@ -462,7 +466,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C8" s="4">
         <v>10</v>
       </c>
@@ -474,7 +478,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C9" s="4">
         <v>15</v>
       </c>
@@ -486,7 +490,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -495,7 +499,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -511,7 +515,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -520,7 +524,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -529,7 +533,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -538,7 +542,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -547,7 +551,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
         <v>0</v>
       </c>
@@ -559,60 +563,60 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>

</xml_diff>

<commit_message>
show in the formula bar only those named ranges that can be selected (#623)
Some named ranges are not-selectable (e.g. referring to a non-continuous area, or to a formula). MS Excel does not show them in the formula bar named ranges selector. This PR changes the Spreadsheet behavior accordingly.

Incorporates the PR #622 by @ianscriven (fixes #621).

Fixes the issue that when a user attempted to select a non-selectable named range it did not get selected.

Contains a workaround for the POI issue https://bz.apache.org/bugzilla/show_bug.cgi?id=61701 that causes IllegalArgumentException when trying to select a named range referring to some formulas.

Jira: SHEET-338
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="3140" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
   <definedNames>
     <definedName name="john">Sheet1!$G$7:$M$16</definedName>
     <definedName name="local" localSheetId="0">Sheet1!$G$2:$H$3</definedName>
+    <definedName name="named_formula">SUM(Sheet1!$C$3:$C$9)</definedName>
     <definedName name="noncont">Sheet1!$19:$19,Sheet1!$21:$21</definedName>
     <definedName name="numbers">Sheet1!$C$3:$C$9</definedName>
     <definedName name="sheet2">Sheet2!$B$3:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -130,13 +131,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -404,19 +408,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -425,7 +429,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="4">
         <v>4</v>
@@ -433,22 +437,22 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C4" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C5" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C6" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C7" s="4">
         <v>9</v>
       </c>
@@ -462,7 +466,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C8" s="4">
         <v>10</v>
       </c>
@@ -474,7 +478,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C9" s="4">
         <v>15</v>
       </c>
@@ -486,7 +490,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -495,7 +499,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -511,7 +515,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -520,7 +524,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -529,7 +533,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -538,7 +542,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -547,7 +551,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
         <v>0</v>
       </c>
@@ -559,60 +563,60 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>

</xml_diff>

<commit_message>
show in the formula bar only those named ranges that can be selected (#627)
Some named ranges are not-selectable (e.g. referring to a non-continuous area, or to a formula). MS Excel does not show them in the formula bar named ranges selector. This PR changes the Spreadsheet behavior accordingly.

Incorporates the PR #622 by @ianscriven (fixes #621).

Fixes the issue that when a user attempted to select a non-selectable named range it did not get selected.

Contains a workaround for the POI issue https://bz.apache.org/bugzilla/show_bug.cgi?id=61701 that causes IllegalArgumentException when trying to select a named range referring to some formulas.

(cherry-picked from 246eeeb from the 1.4 branch + updated the reference screenshot to work in the 2.x branch)

Jira: SHEET-338
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/named_ranges.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="3140" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
   <definedNames>
     <definedName name="john">Sheet1!$G$7:$M$16</definedName>
     <definedName name="local" localSheetId="0">Sheet1!$G$2:$H$3</definedName>
+    <definedName name="named_formula">SUM(Sheet1!$C$3:$C$9)</definedName>
     <definedName name="noncont">Sheet1!$19:$19,Sheet1!$21:$21</definedName>
     <definedName name="numbers">Sheet1!$C$3:$C$9</definedName>
     <definedName name="sheet2">Sheet2!$B$3:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -130,13 +131,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -404,19 +408,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -425,7 +429,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="4">
         <v>4</v>
@@ -433,22 +437,22 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C4" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C5" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C6" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C7" s="4">
         <v>9</v>
       </c>
@@ -462,7 +466,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C8" s="4">
         <v>10</v>
       </c>
@@ -474,7 +478,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C9" s="4">
         <v>15</v>
       </c>
@@ -486,7 +490,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -495,7 +499,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -511,7 +515,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -520,7 +524,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -529,7 +533,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -538,7 +542,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -547,7 +551,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
         <v>0</v>
       </c>
@@ -559,60 +563,60 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>

</xml_diff>